<commit_message>
move Excel reading from COM object to Openpyxl library
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18060" windowHeight="10365"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
+  </definedNames>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -53,12 +61,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -351,23 +354,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <f>SUM(A1:A3)</f>
+        <f t="shared" ref="B1:B18" si="0">SUM(A1:A3)</f>
         <v>6</v>
       </c>
       <c r="C1">
-        <f>SIN(B1*A1^2)</f>
+        <f t="shared" ref="C1:C18" si="1">SIN(B1*A1^2)</f>
         <v>-0.27941549819892586</v>
       </c>
       <c r="D1">
@@ -375,20 +380,20 @@
         <v>-2.2863768173008364E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B18" si="0">SUM(A2:A4)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C18" si="1">SIN(B2*A2^2)</f>
+        <f t="shared" si="1"/>
         <v>-0.99177885344311578</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -401,7 +406,7 @@
         <v>0.92681850541778499</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -414,7 +419,7 @@
         <v>0.9454451549211168</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -427,7 +432,7 @@
         <v>-0.68328372503552359</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -440,7 +445,7 @@
         <v>0.90176229056057366</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -453,7 +458,7 @@
         <v>0.86459689169594789</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -466,7 +471,7 @@
         <v>0.12372268789623808</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -479,7 +484,7 @@
         <v>-0.99975982007864272</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -492,7 +497,7 @@
         <v>0.97060061981194778</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -505,7 +510,7 @@
         <v>0.98352241357378278</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -518,7 +523,7 @@
         <v>-0.91983693466953753</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>13</v>
       </c>
@@ -531,7 +536,7 @@
         <v>-0.90954815110388421</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>14</v>
       </c>
@@ -544,7 +549,7 @@
         <v>-0.9997715643824282</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>15</v>
       </c>
@@ -557,7 +562,7 @@
         <v>-0.71424378349544093</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>16</v>
       </c>
@@ -570,7 +575,7 @@
         <v>-0.44311307948133072</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -583,7 +588,7 @@
         <v>-0.80062916411734009</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -598,6 +603,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -607,9 +617,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -619,8 +634,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improve inherited methods + range api implementation
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="SINUS">Sheet1!$C$1:$C$18</definedName>
-  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -352,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -363,7 +360,7 @@
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -375,12 +372,8 @@
         <f t="shared" ref="C1:C18" si="1">SIN(B1*A1^2)</f>
         <v>-0.27941549819892586</v>
       </c>
-      <c r="D1">
-        <f>LINEST(C1:C18,B1:B18)</f>
-        <v>-2.2863768173008364E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -393,7 +386,7 @@
         <v>-0.99177885344311578</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -406,7 +399,7 @@
         <v>0.92681850541778499</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -419,7 +412,7 @@
         <v>0.9454451549211168</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -432,7 +425,7 @@
         <v>-0.68328372503552359</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -445,7 +438,7 @@
         <v>0.90176229056057366</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -458,7 +451,7 @@
         <v>0.86459689169594789</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -471,7 +464,7 @@
         <v>0.12372268789623808</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -484,7 +477,7 @@
         <v>-0.99975982007864272</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -497,7 +490,7 @@
         <v>0.97060061981194778</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -510,7 +503,7 @@
         <v>0.98352241357378278</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -523,7 +516,7 @@
         <v>-0.91983693466953753</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -536,7 +529,7 @@
         <v>-0.90954815110388421</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -549,7 +542,7 @@
         <v>-0.9997715643824282</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -562,7 +555,7 @@
         <v>-0.71424378349544093</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
introduce data only workbook
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -349,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -360,7 +360,7 @@
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -372,8 +372,12 @@
         <f t="shared" ref="C1:C18" si="1">SIN(B1*A1^2)</f>
         <v>-0.27941549819892586</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <f>LINEST(C1:C18,B1:B18)</f>
+        <v>-2.2863768173008364E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -386,7 +390,7 @@
         <v>-0.99177885344311578</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -399,7 +403,7 @@
         <v>0.92681850541778499</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -412,7 +416,7 @@
         <v>0.9454451549211168</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -425,7 +429,7 @@
         <v>-0.68328372503552359</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -438,7 +442,7 @@
         <v>0.90176229056057366</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -451,7 +455,7 @@
         <v>0.86459689169594789</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -464,7 +468,7 @@
         <v>0.12372268789623808</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -477,7 +481,7 @@
         <v>-0.99975982007864272</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -490,7 +494,7 @@
         <v>0.97060061981194778</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -503,7 +507,7 @@
         <v>0.98352241357378278</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -516,7 +520,7 @@
         <v>-0.91983693466953753</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>13</v>
       </c>
@@ -529,7 +533,7 @@
         <v>-0.90954815110388421</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>14</v>
       </c>
@@ -542,7 +546,7 @@
         <v>-0.9997715643824282</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>15</v>
       </c>
@@ -555,7 +559,7 @@
         <v>-0.71424378349544093</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>16</v>
       </c>

</xml_diff>